<commit_message>
Refine experiments master data, combine content with variables
</commit_message>
<xml_diff>
--- a/03_Codebase/res/experiments_config/bias_params.xlsx
+++ b/03_Codebase/res/experiments_config/bias_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mAx/Documents/Master/04/Master_Thesis/03_Codebase/res/experiments_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A525A2-A091-5047-A786-75F8F1912A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E99B26E-5C8F-D742-8D76-92C34CB652F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13760" yWindow="3680" windowWidth="29860" windowHeight="19000" xr2:uid="{956F8307-781D-7F48-A524-B2B719850CE6}"/>
+    <workbookView xWindow="19180" yWindow="3920" windowWidth="29860" windowHeight="19000" xr2:uid="{956F8307-781D-7F48-A524-B2B719850CE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>bias</t>
   </si>
   <si>
-    <t>experiment</t>
-  </si>
-  <si>
     <t>content</t>
   </si>
   <si>
@@ -59,13 +56,22 @@
     <t>odd_numbers</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
     <t>{"this": 12, "that": 22}</t>
+  </si>
+  <si>
+    <t>{"this": 841758, "that": 1341}</t>
+  </si>
+  <si>
+    <t>bias_id</t>
+  </si>
+  <si>
+    <t>experiment_type</t>
+  </si>
+  <si>
+    <t>Let's test this and whether it is different to that.</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -101,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -437,59 +444,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881B30BE-3872-014C-BA65-F47A6EDA683D}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add target choice to bias parameters
</commit_message>
<xml_diff>
--- a/03_Codebase/res/experiments_config/bias_params.xlsx
+++ b/03_Codebase/res/experiments_config/bias_params.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mAx/Documents/Master/04/Master_Thesis/03_Codebase/res/experiments_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E99B26E-5C8F-D742-8D76-92C34CB652F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8D5C04-236C-B04F-A28E-A7799EE4858B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19180" yWindow="3920" windowWidth="29860" windowHeight="19000" xr2:uid="{956F8307-781D-7F48-A524-B2B719850CE6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>bias</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>target_choice</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -107,9 +116,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -444,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881B30BE-3872-014C-BA65-F47A6EDA683D}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,7 +466,7 @@
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -474,9 +482,12 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>10</v>
       </c>
       <c r="B2" t="s">
@@ -491,8 +502,11 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>11</v>
       </c>
@@ -508,8 +522,11 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>12</v>
       </c>
@@ -521,6 +538,9 @@
       </c>
       <c r="D4" t="s">
         <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>